<commit_message>
Update event announcement template to have correct formatting for lines to 100
</commit_message>
<xml_diff>
--- a/assets/ohlaska_pan_hlavni.xlsx
+++ b/assets/ohlaska_pan_hlavni.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE1B914-FC46-46B8-9EC8-E1A2F344882D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D214F2-364A-4198-AA14-D2D68FB13949}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8925" tabRatio="264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" tabRatio="264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ohláška" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -243,31 +243,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -852,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -930,7 +905,7 @@
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="26"/>
+      <c r="F11" s="19"/>
       <c r="G11"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -957,17 +932,17 @@
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
-      <c r="C19" s="26"/>
+      <c r="C19" s="19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
@@ -1076,9 +1051,9 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="13"/>
-      <c r="B33" s="18"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="15"/>
-      <c r="D33" s="18"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="16"/>
       <c r="G33" s="17"/>
@@ -1096,9 +1071,9 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="13"/>
-      <c r="B35" s="18"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="15"/>
-      <c r="D35" s="19"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="16"/>
       <c r="G35" s="17"/>
@@ -1106,9 +1081,9 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
-      <c r="B36" s="20"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="20"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="16"/>
       <c r="G36" s="17"/>
@@ -1126,9 +1101,9 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="13"/>
-      <c r="B38" s="21"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="15"/>
-      <c r="D38" s="21"/>
+      <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="16"/>
       <c r="G38" s="17"/>
@@ -1136,9 +1111,9 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="13"/>
-      <c r="B39" s="18"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="15"/>
-      <c r="D39" s="18"/>
+      <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="16"/>
       <c r="G39" s="17"/>
@@ -1156,9 +1131,9 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="13"/>
-      <c r="B41" s="20"/>
+      <c r="B41" s="14"/>
       <c r="C41" s="15"/>
-      <c r="D41" s="20"/>
+      <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
@@ -1166,9 +1141,9 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="13"/>
-      <c r="B42" s="20"/>
+      <c r="B42" s="14"/>
       <c r="C42" s="15"/>
-      <c r="D42" s="20"/>
+      <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="16"/>
       <c r="G42" s="17"/>
@@ -1176,52 +1151,820 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="13"/>
-      <c r="B43" s="20"/>
+      <c r="B43" s="14"/>
       <c r="C43" s="15"/>
-      <c r="D43" s="20"/>
+      <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="22"/>
-      <c r="B44" s="20"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="15"/>
-      <c r="D44" s="20"/>
+      <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
       <c r="H44" s="12"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
-      <c r="B45" s="20"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="14"/>
       <c r="C45" s="15"/>
-      <c r="D45" s="13"/>
+      <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="23"/>
+      <c r="G45" s="17"/>
       <c r="H45" s="12"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="20"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="16"/>
       <c r="G46" s="17"/>
       <c r="H46" s="12"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="13"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="17"/>
       <c r="H47" s="12"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="13"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="17"/>
       <c r="H48" s="12"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="13"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="17"/>
       <c r="H49" s="12"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="13"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="13"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="17"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="13"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="17"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="13"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="17"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="13"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="17"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="13"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="17"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="13"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="17"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="13"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="17"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="13"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="17"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="13"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="17"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="13"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="17"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="13"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="17"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="13"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="13"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="13"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="17"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" s="13"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="17"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="13"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="13"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="17"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="13"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="17"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="13"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="15"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="17"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="13"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="15"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="17"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="13"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="15"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="17"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="13"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="17"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="13"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="17"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="13"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="17"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="13"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="15"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="17"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" s="13"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="17"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="13"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="15"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="17"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="13"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="15"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="17"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="13"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="17"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="13"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="15"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="17"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="13"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="17"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="13"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="15"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="17"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="13"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="15"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="17"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" s="13"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="15"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="17"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="13"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="15"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="17"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" s="13"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="17"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" s="13"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="15"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="17"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" s="13"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="15"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="17"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" s="13"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="15"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="17"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" s="13"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="15"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="17"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" s="13"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="15"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="17"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" s="13"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="17"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" s="13"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="15"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="17"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" s="13"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="17"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" s="13"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="17"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" s="13"/>
+      <c r="B96" s="14"/>
+      <c r="C96" s="15"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="17"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="13"/>
+      <c r="B97" s="14"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="17"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="13"/>
+      <c r="B98" s="14"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="17"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="13"/>
+      <c r="B99" s="14"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="17"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" s="13"/>
+      <c r="B100" s="14"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="17"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" s="13"/>
+      <c r="B101" s="14"/>
+      <c r="C101" s="15"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="17"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" s="13"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="17"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="13"/>
+      <c r="B103" s="14"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="17"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="13"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="17"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="13"/>
+      <c r="B105" s="14"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="17"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="13"/>
+      <c r="B106" s="14"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="17"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" s="13"/>
+      <c r="B107" s="14"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="17"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="13"/>
+      <c r="B108" s="14"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="17"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A109" s="13"/>
+      <c r="B109" s="14"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="17"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="13"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="15"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="17"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="13"/>
+      <c r="B111" s="14"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="17"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="13"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="17"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="13"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="15"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="17"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="13"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="17"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="13"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="17"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="13"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="16"/>
+      <c r="G116" s="17"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="13"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="17"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="13"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="15"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="16"/>
+      <c r="G118" s="17"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="13"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="16"/>
+      <c r="G119" s="17"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="13"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="17"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" s="13"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="16"/>
+      <c r="G121" s="17"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" s="13"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="15"/>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="16"/>
+      <c r="G122" s="17"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" s="13"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="15"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="16"/>
+      <c r="G123" s="17"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="13"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="15"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="16"/>
+      <c r="G124" s="17"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" s="13"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="16"/>
+      <c r="G125" s="17"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" s="13"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="15"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="17"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" s="13"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="15"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="17"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" s="13"/>
+      <c r="B128" s="14"/>
+      <c r="C128" s="15"/>
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="17"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="13"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="15"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+      <c r="F129" s="16"/>
+      <c r="G129" s="17"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="13"/>
+      <c r="B130" s="14"/>
+      <c r="C130" s="15"/>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
+      <c r="F130" s="16"/>
+      <c r="G130" s="17"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="13"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="15"/>
+      <c r="D131" s="14"/>
+      <c r="E131" s="14"/>
+      <c r="F131" s="16"/>
+      <c r="G131" s="17"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" s="13"/>
+      <c r="B132" s="14"/>
+      <c r="C132" s="15"/>
+      <c r="D132" s="14"/>
+      <c r="E132" s="14"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="17"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>